<commit_message>
feat: encrypt successfully for one file
</commit_message>
<xml_diff>
--- a/EncryptSample/ExcelContainer/NameAndPassword.xlsx
+++ b/EncryptSample/ExcelContainer/NameAndPassword.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\self-Practice\testContainer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\self-Practice\BackEnd\EncryptSample\EncryptSample\ExcelContainer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F102800A-7100-4DFF-A33A-D492FFB4F1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D28AF2-D738-492E-8164-347EEC975B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5E516563-BA83-49D1-B48A-DFA36EEC2E61}"/>
   </bookViews>
@@ -35,19 +35,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>林小美</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B123456</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>王曉明</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>林小美</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>A12345</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B23456</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -436,12 +436,12 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>

</xml_diff>